<commit_message>
Gerador de Perfis v2.2
</commit_message>
<xml_diff>
--- a/perfis_generated_openpyxl.xlsx
+++ b/perfis_generated_openpyxl.xlsx
@@ -454,11 +454,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Larissa Correia</t>
+          <t>Tatiana Dias</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -467,7 +467,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>128.560.030-44</t>
+          <t>656.432.680-78</t>
         </is>
       </c>
     </row>
@@ -477,11 +477,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Ana Andrade</t>
+          <t>Vanessa Ramos Gouveia</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -490,7 +490,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>998.572.610-35</t>
+          <t>400.161.510-03</t>
         </is>
       </c>
     </row>
@@ -500,20 +500,20 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Luciano Dias</t>
+          <t>Mariana Machado</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>350.903.780-45</t>
+          <t>204.128.760-86</t>
         </is>
       </c>
     </row>
@@ -523,20 +523,20 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Luis Rocha</t>
+          <t>Priscila Ribeira</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>311.578.550-08</t>
+          <t>348.777.810-64</t>
         </is>
       </c>
     </row>
@@ -546,20 +546,20 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Patrícia Rocha</t>
+          <t>Giovanni Correia</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>436.700.700-60</t>
+          <t>246.641.120-25</t>
         </is>
       </c>
     </row>
@@ -569,11 +569,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Amanda Pinto Rodrigues</t>
+          <t>Ana Mendes Nunes</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -582,7 +582,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>586.857.760-40</t>
+          <t>745.361.160-10</t>
         </is>
       </c>
     </row>
@@ -592,20 +592,20 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Wagner Moraes</t>
+          <t>Rosana Ferreira</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>112.048.580-04</t>
+          <t>904.016.070-89</t>
         </is>
       </c>
     </row>
@@ -615,11 +615,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Leonardo Dias</t>
+          <t>Alexandre Mendes</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -628,7 +628,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>658.242.000-33</t>
+          <t>727.704.580-78</t>
         </is>
       </c>
     </row>
@@ -638,11 +638,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Wagner Rodrigues</t>
+          <t>Raul Pessoa</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -651,7 +651,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>592.179.800-21</t>
+          <t>572.522.700-68</t>
         </is>
       </c>
     </row>
@@ -661,11 +661,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Bruno Castro</t>
+          <t>Pedro Moraes</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -674,7 +674,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>133.511.280-45</t>
+          <t>696.594.090-52</t>
         </is>
       </c>
     </row>
@@ -684,11 +684,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Larissa Correia</t>
+          <t>Larissa Gonçalves</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -697,7 +697,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>278.894.780-11</t>
+          <t>290.705.390-63</t>
         </is>
       </c>
     </row>
@@ -707,20 +707,20 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Felipe Santos</t>
+          <t>Tânia Nogueira</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>795.211.790-40</t>
+          <t>832.552.030-23</t>
         </is>
       </c>
     </row>
@@ -730,20 +730,20 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Ricardo Nunes</t>
+          <t>Larissa Ribeira Correia</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>992.832.160-40</t>
+          <t>900.193.570-28</t>
         </is>
       </c>
     </row>
@@ -753,20 +753,20 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Elias Ribeira</t>
+          <t>Karla Monteiro</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>091.565.950-69</t>
+          <t>680.751.920-60</t>
         </is>
       </c>
     </row>
@@ -776,20 +776,20 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Tatiana Alves Rocha</t>
+          <t>César Pereira</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>650.179.490-03</t>
+          <t>924.562.250-90</t>
         </is>
       </c>
     </row>
@@ -799,20 +799,20 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Natália Barbosa</t>
+          <t>Rafael Nunes</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>130.116.240-03</t>
+          <t>883.764.850-24</t>
         </is>
       </c>
     </row>
@@ -822,11 +822,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Amanda Vieira Vieira</t>
+          <t>Márcia Freitas</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -835,7 +835,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>926.675.820-55</t>
+          <t>445.968.720-82</t>
         </is>
       </c>
     </row>
@@ -845,11 +845,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Carlos Gomes</t>
+          <t>Gilberto Freitas</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -858,7 +858,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>494.268.340-87</t>
+          <t>728.381.180-05</t>
         </is>
       </c>
     </row>
@@ -868,20 +868,20 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Cristina Azevedo</t>
+          <t>Roberto Lopes</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>151.772.320-50</t>
+          <t>776.368.110-14</t>
         </is>
       </c>
     </row>
@@ -891,20 +891,20 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Cecília Borges</t>
+          <t>Wagner Sousa</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>196.538.240-15</t>
+          <t>742.029.430-58</t>
         </is>
       </c>
     </row>
@@ -914,20 +914,20 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Patrícia Ramos</t>
+          <t>Diego Alves</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>330.369.640-37</t>
+          <t>081.894.660-11</t>
         </is>
       </c>
     </row>
@@ -937,7 +937,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Roberta Costa Lima</t>
+          <t>Thais Gouveia</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -950,7 +950,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>885.390.700-22</t>
+          <t>663.231.940-82</t>
         </is>
       </c>
     </row>
@@ -960,20 +960,20 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Nathalia Silveira</t>
+          <t>Raul Carvalho</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>746.836.110-07</t>
+          <t>846.727.520-03</t>
         </is>
       </c>
     </row>
@@ -983,20 +983,20 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Gustavo Gonçalves</t>
+          <t>Mônica Martins</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>383.559.150-97</t>
+          <t>831.819.160-99</t>
         </is>
       </c>
     </row>
@@ -1006,11 +1006,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Mariana Vieira</t>
+          <t>Cristina Andrade</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1019,7 +1019,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>956.066.960-53</t>
+          <t>092.119.920-10</t>
         </is>
       </c>
     </row>
@@ -1029,20 +1029,20 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Tatiane Gomes Barbosa</t>
+          <t>Larissa Machado</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Não-Binário</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>164.435.770-43</t>
+          <t>320.084.090-07</t>
         </is>
       </c>
     </row>
@@ -1052,20 +1052,20 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Vanessa Barros</t>
+          <t>Alberto Carvalho Martins</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>918.560.100-40</t>
+          <t>894.456.690-96</t>
         </is>
       </c>
     </row>
@@ -1075,20 +1075,20 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Larissa Ferreira</t>
+          <t>Isaac Pinto</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>051.286.520-50</t>
+          <t>803.496.170-15</t>
         </is>
       </c>
     </row>
@@ -1098,20 +1098,20 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Wagner Araújo</t>
+          <t>Thais Freitas Oliveira</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>534.456.140-75</t>
+          <t>305.147.070-89</t>
         </is>
       </c>
     </row>
@@ -1121,11 +1121,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Valéria Nunes</t>
+          <t>Isabela Rocha</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1134,7 +1134,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>555.892.370-92</t>
+          <t>772.344.590-30</t>
         </is>
       </c>
     </row>
@@ -1144,11 +1144,11 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>José Santana</t>
+          <t>Alexandre Carvalho Cavalcanti</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1157,7 +1157,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>374.976.080-29</t>
+          <t>250.493.920-55</t>
         </is>
       </c>
     </row>
@@ -1167,11 +1167,11 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Larissa Lima</t>
+          <t>Larissa Fernandes</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1180,7 +1180,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>566.748.670-98</t>
+          <t>871.752.910-78</t>
         </is>
       </c>
     </row>
@@ -1190,20 +1190,20 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Sérgio Ribeira</t>
+          <t>Thais Pereira</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>169.314.850-16</t>
+          <t>331.372.520-16</t>
         </is>
       </c>
     </row>
@@ -1213,20 +1213,20 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Nathalia Nogueira</t>
+          <t>Luis Campos</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>573.070.210-80</t>
+          <t>805.941.410-01</t>
         </is>
       </c>
     </row>
@@ -1236,11 +1236,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Roberto Costa Pereira</t>
+          <t>Vinícius Silva</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1249,7 +1249,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>408.409.710-10</t>
+          <t>309.926.160-26</t>
         </is>
       </c>
     </row>
@@ -1259,20 +1259,20 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Ricardo Costa Nunes</t>
+          <t>Vanessa Gouveia</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>036.355.290-10</t>
+          <t>714.139.540-73</t>
         </is>
       </c>
     </row>
@@ -1282,20 +1282,20 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Sergio Castro</t>
+          <t>Simone Pereira Moraes</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>280.170.780-56</t>
+          <t>944.394.550-93</t>
         </is>
       </c>
     </row>
@@ -1305,11 +1305,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Helena Oliveira</t>
+          <t>Aline Gomes</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1318,7 +1318,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>519.115.730-39</t>
+          <t>208.359.290-51</t>
         </is>
       </c>
     </row>
@@ -1328,20 +1328,20 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Nathalia Dias Costa</t>
+          <t>Gilberto Dias</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>079.774.500-97</t>
+          <t>780.022.750-20</t>
         </is>
       </c>
     </row>
@@ -1351,11 +1351,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Vanessa Almeida Nascimento</t>
+          <t>Regina Gouveia</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>511.553.350-23</t>
+          <t>325.064.500-17</t>
         </is>
       </c>
     </row>
@@ -1374,20 +1374,20 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Andressa Gonçalves Borges</t>
+          <t>Vitor Castro</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>405.655.000-07</t>
+          <t>169.068.870-09</t>
         </is>
       </c>
     </row>
@@ -1397,11 +1397,11 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Luis Rocha</t>
+          <t>Caio Gonçalves</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>227.436.280-73</t>
+          <t>035.565.730-91</t>
         </is>
       </c>
     </row>
@@ -1420,11 +1420,11 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Thais Barbosa</t>
+          <t>Isabela Cardoso</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -1433,7 +1433,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>775.060.700-57</t>
+          <t>319.286.150-90</t>
         </is>
       </c>
     </row>
@@ -1443,11 +1443,11 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Paulo Monteiro</t>
+          <t>César Costa Lima</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -1456,7 +1456,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>324.028.120-10</t>
+          <t>124.503.320-49</t>
         </is>
       </c>
     </row>
@@ -1466,20 +1466,20 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Elaine Campos</t>
+          <t>Fernando Nogueira</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>631.729.940-40</t>
+          <t>589.911.280-84</t>
         </is>
       </c>
     </row>
@@ -1489,11 +1489,11 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Raul Almeida</t>
+          <t>Pedro Almeida</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -1502,7 +1502,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>313.661.630-87</t>
+          <t>394.420.650-92</t>
         </is>
       </c>
     </row>
@@ -1512,20 +1512,20 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Eduarda Moraes</t>
+          <t>Guilherme Fernandes</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>621.696.750-94</t>
+          <t>821.602.710-98</t>
         </is>
       </c>
     </row>
@@ -1535,20 +1535,20 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Regina Gonçalves</t>
+          <t>Vicente Silveira</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>557.494.420-04</t>
+          <t>466.837.800-30</t>
         </is>
       </c>
     </row>
@@ -1558,20 +1558,20 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Paulo Pessoa</t>
+          <t>Sueli Freitas</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>564.077.540-89</t>
+          <t>311.051.900-30</t>
         </is>
       </c>
     </row>
@@ -1581,20 +1581,20 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Vinícius Moraes</t>
+          <t>Aline Cardoso Gomes</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>403.111.360-95</t>
+          <t>965.836.480-24</t>
         </is>
       </c>
     </row>
@@ -1604,20 +1604,20 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>João Freitas</t>
+          <t>Tatiane Silva</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>350.857.220-00</t>
+          <t>751.278.980-71</t>
         </is>
       </c>
     </row>
@@ -1627,11 +1627,11 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Isabela Oliveira</t>
+          <t>Eduarda Cavalcanti</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -1640,7 +1640,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>553.572.830-60</t>
+          <t>202.330.900-02</t>
         </is>
       </c>
     </row>
@@ -1650,20 +1650,20 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Isabela Mendes Nascimento</t>
+          <t>Renato Ramos</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>300.393.380-96</t>
+          <t>189.749.740-70</t>
         </is>
       </c>
     </row>
@@ -1673,11 +1673,11 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Diego Pessoa</t>
+          <t>Felipe Martins</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -1686,7 +1686,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>503.586.400-67</t>
+          <t>300.211.640-88</t>
         </is>
       </c>
     </row>
@@ -1696,11 +1696,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Sergio Sousa Nascimento</t>
+          <t>Vinícius Carvalho</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>140.973.000-08</t>
+          <t>376.031.040-09</t>
         </is>
       </c>
     </row>
@@ -1719,20 +1719,20 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Ronaldo Nascimento</t>
+          <t>Simone Carvalho Pereira</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807.650.050-85</t>
+          <t>535.750.180-73</t>
         </is>
       </c>
     </row>
@@ -1742,11 +1742,11 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Roberto Freitas</t>
+          <t>Elias Almeida</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -1755,7 +1755,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>703.949.780-80</t>
+          <t>743.153.350-02</t>
         </is>
       </c>
     </row>
@@ -1765,11 +1765,11 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Arnaldo Santos Pinto</t>
+          <t>Giovanni Borges</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>166.374.890-00</t>
+          <t>943.818.610-78</t>
         </is>
       </c>
     </row>
@@ -1788,20 +1788,20 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Mariana Pereira</t>
+          <t>Pedro Rocha</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>886.512.890-90</t>
+          <t>452.355.230-40</t>
         </is>
       </c>
     </row>
@@ -1811,11 +1811,11 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Eduardo Monteiro</t>
+          <t>Sérgio Cavalcanti</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -1824,7 +1824,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>773.577.350-10</t>
+          <t>717.686.110-25</t>
         </is>
       </c>
     </row>
@@ -1834,20 +1834,20 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Mônica Santos</t>
+          <t>Eduardo Lopes</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>863.934.250-40</t>
+          <t>757.827.650-62</t>
         </is>
       </c>
     </row>
@@ -1857,20 +1857,20 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Roberto Ramos</t>
+          <t>Fernanda Correia</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>887.315.700-97</t>
+          <t>906.260.300-99</t>
         </is>
       </c>
     </row>
@@ -1880,11 +1880,11 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Raul Gonçalves Cavalcanti</t>
+          <t>Ricardo Ferreira</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -1893,7 +1893,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>415.923.130-60</t>
+          <t>002.985.470-90</t>
         </is>
       </c>
     </row>
@@ -1903,11 +1903,11 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Larissa Pereira Ribeira</t>
+          <t>Luiza Almeida</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -1916,7 +1916,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>881.806.120-82</t>
+          <t>182.138.720-10</t>
         </is>
       </c>
     </row>
@@ -1926,20 +1926,20 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Larissa Gonçalves</t>
+          <t>Álvaro Dias</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>317.873.910-60</t>
+          <t>648.541.020-12</t>
         </is>
       </c>
     </row>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Luiza Costa</t>
+          <t>Vanessa Alves</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -1962,7 +1962,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>810.540.320-09</t>
+          <t>281.337.150-59</t>
         </is>
       </c>
     </row>
@@ -1972,11 +1972,11 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Pedro Ribeira</t>
+          <t>Arnaldo Rodrigues</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>360.536.620-11</t>
+          <t>716.194.570-40</t>
         </is>
       </c>
     </row>
@@ -1995,20 +1995,20 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Flávia Pires</t>
+          <t>Arnaldo Nogueira</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>852.782.450-77</t>
+          <t>307.502.370-15</t>
         </is>
       </c>
     </row>
@@ -2018,11 +2018,11 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Vinícius Alves Santos</t>
+          <t>Gustavo Lopes</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -2031,7 +2031,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>403.781.790-04</t>
+          <t>266.920.320-59</t>
         </is>
       </c>
     </row>
@@ -2041,20 +2041,20 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Vitor Mendes Carvalho</t>
+          <t>Vanessa Carvalho</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>019.963.050-00</t>
+          <t>729.210.190-94</t>
         </is>
       </c>
     </row>
@@ -2064,11 +2064,11 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Patrícia Ramos</t>
+          <t>Karla Santana</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>899.860.840-59</t>
+          <t>204.801.870-02</t>
         </is>
       </c>
     </row>
@@ -2087,11 +2087,11 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Eduarda Gonçalves</t>
+          <t>Camila Ramos</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -2100,7 +2100,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>040.500.910-03</t>
+          <t>112.591.860-83</t>
         </is>
       </c>
     </row>
@@ -2110,20 +2110,20 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Leticia Nascimento</t>
+          <t>André Gomes</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>508.862.350-06</t>
+          <t>320.623.620-72</t>
         </is>
       </c>
     </row>
@@ -2133,20 +2133,20 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Mariana Fernandes</t>
+          <t>Ricardo Gomes Cardoso</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>218.861.990-00</t>
+          <t>526.980.810-23</t>
         </is>
       </c>
     </row>
@@ -2156,11 +2156,11 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Felipe Rocha</t>
+          <t>Miguel Pessoa</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>569.844.620-29</t>
+          <t>805.205.880-53</t>
         </is>
       </c>
     </row>
@@ -2179,20 +2179,20 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Caio Lima Pinto</t>
+          <t>Simone Ferreira</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>652.988.100-04</t>
+          <t>310.712.990-93</t>
         </is>
       </c>
     </row>
@@ -2202,20 +2202,20 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Valéria Pereira</t>
+          <t>Raul Pinto</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>402.116.420-02</t>
+          <t>708.265.780-39</t>
         </is>
       </c>
     </row>
@@ -2225,11 +2225,11 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Eduardo Silva</t>
+          <t>João Nunes</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -2238,7 +2238,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>970.284.280-87</t>
+          <t>287.536.000-02</t>
         </is>
       </c>
     </row>
@@ -2248,20 +2248,20 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Aline Costa</t>
+          <t>Elaine Silveira</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Não-Binário</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>912.534.740-36</t>
+          <t>358.127.080-37</t>
         </is>
       </c>
     </row>
@@ -2271,11 +2271,11 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Nathalia Lima Vieira</t>
+          <t>Tatiana Andrade</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -2284,7 +2284,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>056.487.470-12</t>
+          <t>808.775.160-49</t>
         </is>
       </c>
     </row>
@@ -2294,20 +2294,20 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Wagner Cardoso Mendes</t>
+          <t>Samuel Gomes</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Não-Binário</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>977.773.370-41</t>
+          <t>871.555.900-96</t>
         </is>
       </c>
     </row>
@@ -2317,20 +2317,20 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Guilherme Campos</t>
+          <t>Andressa Pereira</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>497.128.440-05</t>
+          <t>525.044.160-24</t>
         </is>
       </c>
     </row>
@@ -2340,20 +2340,20 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Geraldo Ribeira</t>
+          <t>Mariana Campos</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>361.428.040-32</t>
+          <t>978.637.130-56</t>
         </is>
       </c>
     </row>
@@ -2363,11 +2363,11 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Tatiana Barbosa</t>
+          <t>Rosana Gonçalves</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -2376,7 +2376,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>998.446.980-81</t>
+          <t>195.135.820-19</t>
         </is>
       </c>
     </row>
@@ -2386,11 +2386,11 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Marcelo Machado</t>
+          <t>Giovanni Freitas Pereira</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -2399,7 +2399,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>407.303.910-51</t>
+          <t>577.443.230-09</t>
         </is>
       </c>
     </row>
@@ -2409,11 +2409,11 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Elias Ribeiro</t>
+          <t>Paulo Vieira</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -2422,7 +2422,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>641.110.930-35</t>
+          <t>572.074.200-05</t>
         </is>
       </c>
     </row>
@@ -2432,11 +2432,11 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Leticia Barros</t>
+          <t>Regina Moraes</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -2445,7 +2445,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>255.698.390-62</t>
+          <t>027.700.850-69</t>
         </is>
       </c>
     </row>
@@ -2455,20 +2455,20 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Larissa Nascimento</t>
+          <t>Sérgio Mendes</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>148.621.280-84</t>
+          <t>549.265.000-94</t>
         </is>
       </c>
     </row>
@@ -2478,20 +2478,20 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Fernanda Moraes</t>
+          <t>Roberto Dias</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>453.361.410-89</t>
+          <t>949.447.530-55</t>
         </is>
       </c>
     </row>
@@ -2501,11 +2501,11 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Vanessa Gomes</t>
+          <t>Jéssica Sousa</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -2514,7 +2514,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>180.097.540-64</t>
+          <t>498.854.390-05</t>
         </is>
       </c>
     </row>
@@ -2524,20 +2524,20 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Eduarda Santana</t>
+          <t>Eduardo Lopes</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>750.989.650-98</t>
+          <t>529.643.730-60</t>
         </is>
       </c>
     </row>
@@ -2547,20 +2547,20 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Isabela Pinto Melo</t>
+          <t>Alberto Araújo</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>335.490.470-45</t>
+          <t>998.879.540-80</t>
         </is>
       </c>
     </row>
@@ -2570,11 +2570,11 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Rosana Rodrigues</t>
+          <t>Sandra Melo</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -2583,7 +2583,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>806.735.390-59</t>
+          <t>144.699.740-56</t>
         </is>
       </c>
     </row>
@@ -2593,20 +2593,20 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Vanessa Ribeiro</t>
+          <t>Larissa Moraes</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Não-Binário</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>440.474.690-33</t>
+          <t>263.488.890-25</t>
         </is>
       </c>
     </row>
@@ -2616,20 +2616,20 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Thiago Gouveia Moraes</t>
+          <t>Karla Lima</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Não-Binário</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>921.491.710-82</t>
+          <t>856.443.660-49</t>
         </is>
       </c>
     </row>
@@ -2639,11 +2639,11 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Larissa Dias</t>
+          <t>Carla Pereira</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
@@ -2652,7 +2652,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>443.064.410-16</t>
+          <t>783.669.390-22</t>
         </is>
       </c>
     </row>
@@ -2662,11 +2662,11 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Fernanda Pereira</t>
+          <t>Mariana Machado</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
@@ -2675,7 +2675,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>117.958.270-50</t>
+          <t>456.825.350-06</t>
         </is>
       </c>
     </row>
@@ -2685,20 +2685,20 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Ronaldo Fernandes Andrade</t>
+          <t>Luiza Araújo</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>005.675.160-59</t>
+          <t>055.054.560-30</t>
         </is>
       </c>
     </row>
@@ -2708,11 +2708,11 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Anderson Nogueira</t>
+          <t>André Carvalho Sousa</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
@@ -2721,7 +2721,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>832.087.010-04</t>
+          <t>595.307.030-66</t>
         </is>
       </c>
     </row>
@@ -2731,11 +2731,11 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Rosana Lima</t>
+          <t>Bianca Correia Nunes</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
@@ -2744,7 +2744,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>217.517.340-21</t>
+          <t>564.388.270-10</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Gerador de Perfis c2.3
</commit_message>
<xml_diff>
--- a/perfis_generated_openpyxl.xlsx
+++ b/perfis_generated_openpyxl.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,6 +447,11 @@
           <t>CPF</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>CEP</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -454,11 +459,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Tatiana Dias</t>
+          <t>Márcia Dias Pires</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -467,7 +472,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>656.432.680-78</t>
+          <t>454.730.420-31</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>457480213</t>
         </is>
       </c>
     </row>
@@ -477,20 +487,25 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Vanessa Ramos Gouveia</t>
+          <t>Isaac Moraes</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>400.161.510-03</t>
+          <t>731.736.010-41</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>718388663</t>
         </is>
       </c>
     </row>
@@ -500,20 +515,25 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Mariana Machado</t>
+          <t>Raul Barbosa Pereira</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>204.128.760-86</t>
+          <t>734.122.850-48</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>375740544</t>
         </is>
       </c>
     </row>
@@ -523,20 +543,25 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Priscila Ribeira</t>
+          <t>Felipe Campos Correia</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>348.777.810-64</t>
+          <t>464.763.310-19</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>840482879</t>
         </is>
       </c>
     </row>
@@ -546,20 +571,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Giovanni Correia</t>
+          <t>Rosana Sousa</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>246.641.120-25</t>
+          <t>888.499.980-40</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>473030048</t>
         </is>
       </c>
     </row>
@@ -569,11 +599,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ana Mendes Nunes</t>
+          <t>Thais Martins</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -582,7 +612,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>745.361.160-10</t>
+          <t>035.001.300-46</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>807669998</t>
         </is>
       </c>
     </row>
@@ -592,11 +627,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Rosana Ferreira</t>
+          <t>Priscila Sousa</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -605,7 +640,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>904.016.070-89</t>
+          <t>249.074.070-92</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>215971588</t>
         </is>
       </c>
     </row>
@@ -615,20 +655,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Alexandre Mendes</t>
+          <t>Mariana Lopes</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>727.704.580-78</t>
+          <t>130.928.250-12</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>570050630</t>
         </is>
       </c>
     </row>
@@ -638,11 +683,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Raul Pessoa</t>
+          <t>Felipe Pereira</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -651,7 +696,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>572.522.700-68</t>
+          <t>700.595.730-07</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>026607922</t>
         </is>
       </c>
     </row>
@@ -661,20 +711,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Pedro Moraes</t>
+          <t>Ana Gomes</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>696.594.090-52</t>
+          <t>954.247.220-08</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>770449243</t>
         </is>
       </c>
     </row>
@@ -684,11 +739,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Larissa Gonçalves</t>
+          <t>Regina Costa</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -697,7 +752,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>290.705.390-63</t>
+          <t>235.961.870-95</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>584915628</t>
         </is>
       </c>
     </row>
@@ -707,11 +767,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Tânia Nogueira</t>
+          <t>Jessica Fernandes Correia</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -720,7 +780,12 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>832.552.030-23</t>
+          <t>520.539.070-02</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>060319223</t>
         </is>
       </c>
     </row>
@@ -730,11 +795,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Larissa Ribeira Correia</t>
+          <t>Vanessa Vieira</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -743,7 +808,12 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>900.193.570-28</t>
+          <t>385.240.980-23</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>516677012</t>
         </is>
       </c>
     </row>
@@ -753,7 +823,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Karla Monteiro</t>
+          <t>Elaine Lopes</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -766,7 +836,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>680.751.920-60</t>
+          <t>578.423.140-55</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>982299166</t>
         </is>
       </c>
     </row>
@@ -776,20 +851,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>César Pereira</t>
+          <t>Nathalia Carvalho</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>924.562.250-90</t>
+          <t>073.690.740-80</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>261015531</t>
         </is>
       </c>
     </row>
@@ -799,11 +879,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Rafael Nunes</t>
+          <t>Pedro Nunes</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -812,7 +892,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>883.764.850-24</t>
+          <t>331.416.900-06</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>821956850</t>
         </is>
       </c>
     </row>
@@ -822,20 +907,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Márcia Freitas</t>
+          <t>José Ramos Nogueira</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>445.968.720-82</t>
+          <t>372.826.150-55</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>743077956</t>
         </is>
       </c>
     </row>
@@ -845,20 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Gilberto Freitas</t>
+          <t>Laura Cardoso</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>728.381.180-05</t>
+          <t>134.432.000-79</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>612255228</t>
         </is>
       </c>
     </row>
@@ -868,11 +963,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Roberto Lopes</t>
+          <t>Elias Monteiro</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -881,7 +976,12 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>776.368.110-14</t>
+          <t>946.794.820-60</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>290056748</t>
         </is>
       </c>
     </row>
@@ -891,20 +991,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Wagner Sousa</t>
+          <t>Mariana Carvalho</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>742.029.430-58</t>
+          <t>304.839.560-15</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>375496809</t>
         </is>
       </c>
     </row>
@@ -914,11 +1019,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Diego Alves</t>
+          <t>Diego Pereira Araújo</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -927,7 +1032,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>081.894.660-11</t>
+          <t>498.409.200-90</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>167582780</t>
         </is>
       </c>
     </row>
@@ -937,11 +1047,11 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Thais Gouveia</t>
+          <t>Ana Pereira</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -950,7 +1060,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>663.231.940-82</t>
+          <t>064.624.610-04</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>252755803</t>
         </is>
       </c>
     </row>
@@ -960,11 +1075,11 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Raul Carvalho</t>
+          <t>João Carvalho</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -973,7 +1088,12 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>846.727.520-03</t>
+          <t>465.071.140-14</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>787197619</t>
         </is>
       </c>
     </row>
@@ -983,20 +1103,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Mônica Martins</t>
+          <t>Gilberto Fernandes</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>831.819.160-99</t>
+          <t>162.037.980-53</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>048896358</t>
         </is>
       </c>
     </row>
@@ -1006,11 +1131,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Cristina Andrade</t>
+          <t>Rosana Pinto</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1019,7 +1144,12 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>092.119.920-10</t>
+          <t>804.864.460-69</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>900973832</t>
         </is>
       </c>
     </row>
@@ -1029,20 +1159,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Larissa Machado</t>
+          <t>Miguel Vieira</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>320.084.090-07</t>
+          <t>031.895.000-61</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>842145565</t>
         </is>
       </c>
     </row>
@@ -1052,11 +1187,11 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Alberto Carvalho Martins</t>
+          <t>Alexandre Rodrigues Nunes</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1065,7 +1200,12 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>894.456.690-96</t>
+          <t>694.366.080-20</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>746803141</t>
         </is>
       </c>
     </row>
@@ -1075,11 +1215,11 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Isaac Pinto</t>
+          <t>Fábio Ramos</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1088,7 +1228,12 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>803.496.170-15</t>
+          <t>612.312.490-05</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>794419543</t>
         </is>
       </c>
     </row>
@@ -1098,20 +1243,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Thais Freitas Oliveira</t>
+          <t>Álvaro Lima</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>305.147.070-89</t>
+          <t>972.260.190-35</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>114509439</t>
         </is>
       </c>
     </row>
@@ -1121,11 +1271,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Isabela Rocha</t>
+          <t>Natália Freitas</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1134,7 +1284,12 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>772.344.590-30</t>
+          <t>168.919.910-56</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>122206954</t>
         </is>
       </c>
     </row>
@@ -1144,20 +1299,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Alexandre Carvalho Cavalcanti</t>
+          <t>Thais Melo</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>250.493.920-55</t>
+          <t>880.239.540-32</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>299487657</t>
         </is>
       </c>
     </row>
@@ -1167,11 +1327,11 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Larissa Fernandes</t>
+          <t>Isabela Oliveira</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1180,7 +1340,12 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>871.752.910-78</t>
+          <t>603.222.170-91</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>139423656</t>
         </is>
       </c>
     </row>
@@ -1190,11 +1355,11 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Thais Pereira</t>
+          <t>Mariana Moraes</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1203,7 +1368,12 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>331.372.520-16</t>
+          <t>596.635.520-77</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>388024000</t>
         </is>
       </c>
     </row>
@@ -1213,20 +1383,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Luis Campos</t>
+          <t>Valéria Carvalho</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>805.941.410-01</t>
+          <t>751.568.220-53</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>452742551</t>
         </is>
       </c>
     </row>
@@ -1236,20 +1411,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Vinícius Silva</t>
+          <t>Juliana Oliveira Dias</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>309.926.160-26</t>
+          <t>070.093.130-91</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>857115097</t>
         </is>
       </c>
     </row>
@@ -1259,11 +1439,11 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Vanessa Gouveia</t>
+          <t>Leticia Barbosa</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1272,7 +1452,12 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>714.139.540-73</t>
+          <t>536.448.240-53</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>711540677</t>
         </is>
       </c>
     </row>
@@ -1282,20 +1467,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Simone Pereira Moraes</t>
+          <t>Leandro Nogueira Correia</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>944.394.550-93</t>
+          <t>201.951.320-09</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>280636763</t>
         </is>
       </c>
     </row>
@@ -1305,11 +1495,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Aline Gomes</t>
+          <t>Sandra Mendes Carvalho</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1318,7 +1508,12 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>208.359.290-51</t>
+          <t>355.089.240-35</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>741495615</t>
         </is>
       </c>
     </row>
@@ -1328,20 +1523,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Gilberto Dias</t>
+          <t>Patrícia Gouveia</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>780.022.750-20</t>
+          <t>088.859.160-82</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>244913470</t>
         </is>
       </c>
     </row>
@@ -1351,11 +1551,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Regina Gouveia</t>
+          <t>Simone Lopes</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1364,7 +1564,12 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>325.064.500-17</t>
+          <t>128.180.470-30</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>953229688</t>
         </is>
       </c>
     </row>
@@ -1374,11 +1579,11 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Vitor Castro</t>
+          <t>Carlos Pires Dias</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -1387,7 +1592,12 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>169.068.870-09</t>
+          <t>382.751.550-53</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>244071353</t>
         </is>
       </c>
     </row>
@@ -1397,11 +1607,11 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Caio Gonçalves</t>
+          <t>Vitor Silveira</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -1410,7 +1620,12 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>035.565.730-91</t>
+          <t>189.800.700-47</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>232713647</t>
         </is>
       </c>
     </row>
@@ -1420,20 +1635,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Isabela Cardoso</t>
+          <t>Alberto Barros</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>319.286.150-90</t>
+          <t>277.193.980-09</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>387893829</t>
         </is>
       </c>
     </row>
@@ -1443,20 +1663,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>César Costa Lima</t>
+          <t>Priscila Dias</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>124.503.320-49</t>
+          <t>850.966.420-03</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>449182893</t>
         </is>
       </c>
     </row>
@@ -1466,11 +1691,11 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Fernando Nogueira</t>
+          <t>Luciano Lopes</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -1479,7 +1704,12 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>589.911.280-84</t>
+          <t>831.867.340-96</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>057502054</t>
         </is>
       </c>
     </row>
@@ -1489,11 +1719,11 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Pedro Almeida</t>
+          <t>Luis Lima Gouveia</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -1502,7 +1732,12 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>394.420.650-92</t>
+          <t>559.979.500-42</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>546802468</t>
         </is>
       </c>
     </row>
@@ -1512,11 +1747,11 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Guilherme Fernandes</t>
+          <t>Sergio Carvalho</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -1525,7 +1760,12 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>821.602.710-98</t>
+          <t>309.926.970-00</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>292559043</t>
         </is>
       </c>
     </row>
@@ -1535,20 +1775,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Vicente Silveira</t>
+          <t>Juliana Ferreira Vieira</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>466.837.800-30</t>
+          <t>096.588.340-00</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>908656150</t>
         </is>
       </c>
     </row>
@@ -1558,11 +1803,11 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Sueli Freitas</t>
+          <t>Karla Ferreira</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -1571,7 +1816,12 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>311.051.900-30</t>
+          <t>978.118.970-32</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>916408101</t>
         </is>
       </c>
     </row>
@@ -1581,20 +1831,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Aline Cardoso Gomes</t>
+          <t>Raul Fernandes</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>965.836.480-24</t>
+          <t>478.199.540-35</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>623764319</t>
         </is>
       </c>
     </row>
@@ -1604,11 +1859,11 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Tatiane Silva</t>
+          <t>Carla Freitas</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -1617,7 +1872,12 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>751.278.980-71</t>
+          <t>155.197.750-87</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>024109830</t>
         </is>
       </c>
     </row>
@@ -1627,11 +1887,11 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Eduarda Cavalcanti</t>
+          <t>Patrícia Oliveira</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -1640,7 +1900,12 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>202.330.900-02</t>
+          <t>287.636.970-25</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>418403233</t>
         </is>
       </c>
     </row>
@@ -1650,11 +1915,11 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Renato Ramos</t>
+          <t>Caio Lopes</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -1663,7 +1928,12 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>189.749.740-70</t>
+          <t>223.362.740-78</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>286796187</t>
         </is>
       </c>
     </row>
@@ -1673,20 +1943,25 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Felipe Martins</t>
+          <t>Ana Rodrigues</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Não-Binário</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>300.211.640-88</t>
+          <t>245.758.110-92</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>513688306</t>
         </is>
       </c>
     </row>
@@ -1696,20 +1971,25 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Vinícius Carvalho</t>
+          <t>Simone Dias</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>376.031.040-09</t>
+          <t>552.835.850-77</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>053619195</t>
         </is>
       </c>
     </row>
@@ -1719,20 +1999,25 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Simone Carvalho Pereira</t>
+          <t>André Ramos</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>535.750.180-73</t>
+          <t>273.740.030-99</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>243745272</t>
         </is>
       </c>
     </row>
@@ -1742,20 +2027,25 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Elias Almeida</t>
+          <t>Roberta Costa</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>743.153.350-02</t>
+          <t>734.318.960-30</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>607822680</t>
         </is>
       </c>
     </row>
@@ -1765,11 +2055,11 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Giovanni Borges</t>
+          <t>Armando Castro</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -1778,7 +2068,12 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>943.818.610-78</t>
+          <t>494.679.480-87</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>894400711</t>
         </is>
       </c>
     </row>
@@ -1788,11 +2083,11 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Pedro Rocha</t>
+          <t>Lucas Borges</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -1801,7 +2096,12 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>452.355.230-40</t>
+          <t>071.524.640-22</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>821110625</t>
         </is>
       </c>
     </row>
@@ -1811,11 +2111,11 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Sérgio Cavalcanti</t>
+          <t>Samuel Ferreira</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -1824,7 +2124,12 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>717.686.110-25</t>
+          <t>863.859.560-32</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>031551496</t>
         </is>
       </c>
     </row>
@@ -1834,11 +2139,11 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Eduardo Lopes</t>
+          <t>Guilherme Nunes</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -1847,7 +2152,12 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>757.827.650-62</t>
+          <t>630.573.300-70</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>700093933</t>
         </is>
       </c>
     </row>
@@ -1857,20 +2167,25 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Fernanda Correia</t>
+          <t>Samuel Silva</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>906.260.300-99</t>
+          <t>510.045.570-51</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>701802412</t>
         </is>
       </c>
     </row>
@@ -1880,11 +2195,11 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Ricardo Ferreira</t>
+          <t>Ronaldo Moraes Campos</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -1893,7 +2208,12 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>002.985.470-90</t>
+          <t>450.616.830-56</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>268202430</t>
         </is>
       </c>
     </row>
@@ -1903,11 +2223,11 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Luiza Almeida</t>
+          <t>Carla Martins</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -1916,7 +2236,12 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>182.138.720-10</t>
+          <t>623.701.950-29</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>803609982</t>
         </is>
       </c>
     </row>
@@ -1926,11 +2251,11 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Álvaro Dias</t>
+          <t>Antônio Azevedo</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -1939,7 +2264,12 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>648.541.020-12</t>
+          <t>513.981.970-84</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>396946790</t>
         </is>
       </c>
     </row>
@@ -1949,11 +2279,11 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Vanessa Alves</t>
+          <t>Patrícia Martins</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -1962,7 +2292,12 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>281.337.150-59</t>
+          <t>580.065.400-04</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>697792646</t>
         </is>
       </c>
     </row>
@@ -1972,11 +2307,11 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Arnaldo Rodrigues</t>
+          <t>Thiago Lopes</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -1985,7 +2320,12 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>716.194.570-40</t>
+          <t>637.793.110-70</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>123234102</t>
         </is>
       </c>
     </row>
@@ -1995,20 +2335,25 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Arnaldo Nogueira</t>
+          <t>Cristina Machado</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>307.502.370-15</t>
+          <t>113.391.740-22</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>778409891</t>
         </is>
       </c>
     </row>
@@ -2018,7 +2363,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Gustavo Lopes</t>
+          <t>Leticia Ferreira</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -2026,12 +2371,17 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>266.920.320-59</t>
+          <t>394.850.440-70</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>530521551</t>
         </is>
       </c>
     </row>
@@ -2041,20 +2391,25 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Vanessa Carvalho</t>
+          <t>Carlos Santana</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>729.210.190-94</t>
+          <t>380.183.210-43</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>030598201</t>
         </is>
       </c>
     </row>
@@ -2064,11 +2419,11 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Karla Santana</t>
+          <t>Simone Castro</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -2077,7 +2432,12 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>204.801.870-02</t>
+          <t>532.753.590-88</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>742256244</t>
         </is>
       </c>
     </row>
@@ -2087,11 +2447,11 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Camila Ramos</t>
+          <t>Sandra Araújo</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -2100,7 +2460,12 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>112.591.860-83</t>
+          <t>280.065.700-60</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>258305407</t>
         </is>
       </c>
     </row>
@@ -2110,11 +2475,11 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>André Gomes</t>
+          <t>Vicente Pereira</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -2123,7 +2488,12 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>320.623.620-72</t>
+          <t>713.336.930-36</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>362217362</t>
         </is>
       </c>
     </row>
@@ -2133,11 +2503,11 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Ricardo Gomes Cardoso</t>
+          <t>João Nogueira</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -2146,7 +2516,12 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>526.980.810-23</t>
+          <t>180.264.990-50</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>410084933</t>
         </is>
       </c>
     </row>
@@ -2156,11 +2531,11 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Miguel Pessoa</t>
+          <t>Fernando Freitas</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -2169,7 +2544,12 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>805.205.880-53</t>
+          <t>055.224.730-88</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>990514266</t>
         </is>
       </c>
     </row>
@@ -2179,20 +2559,25 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Simone Ferreira</t>
+          <t>Alexandre Santos Carvalho</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>310.712.990-93</t>
+          <t>531.384.050-96</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>935528450</t>
         </is>
       </c>
     </row>
@@ -2202,11 +2587,11 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Raul Pinto</t>
+          <t>Raul Ribeira</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -2215,7 +2600,12 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>708.265.780-39</t>
+          <t>645.485.780-80</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>847359135</t>
         </is>
       </c>
     </row>
@@ -2225,20 +2615,25 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>João Nunes</t>
+          <t>Larissa Freitas Barbosa</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>287.536.000-02</t>
+          <t>100.413.760-56</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>394664282</t>
         </is>
       </c>
     </row>
@@ -2248,20 +2643,25 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Elaine Silveira</t>
+          <t>Leonardo Lima</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>358.127.080-37</t>
+          <t>246.284.410-49</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>801523246</t>
         </is>
       </c>
     </row>
@@ -2271,11 +2671,11 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Tatiana Andrade</t>
+          <t>Juliana Mendes Lopes</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -2284,7 +2684,12 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>808.775.160-49</t>
+          <t>078.697.430-38</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>734159646</t>
         </is>
       </c>
     </row>
@@ -2294,20 +2699,25 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Samuel Gomes</t>
+          <t>Karla Nogueira Borges</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Não-Binário</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>871.555.900-96</t>
+          <t>241.540.760-78</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>180984797</t>
         </is>
       </c>
     </row>
@@ -2317,11 +2727,11 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Andressa Pereira</t>
+          <t>Karla Nascimento</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -2330,7 +2740,12 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>525.044.160-24</t>
+          <t>563.704.670-06</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>386690200</t>
         </is>
       </c>
     </row>
@@ -2340,11 +2755,11 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Mariana Campos</t>
+          <t>Amanda Moraes</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -2353,7 +2768,12 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>978.637.130-56</t>
+          <t>415.604.520-05</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>124078147</t>
         </is>
       </c>
     </row>
@@ -2363,20 +2783,25 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Rosana Gonçalves</t>
+          <t>Ricardo Gonçalves</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>195.135.820-19</t>
+          <t>898.639.190-20</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>331894100</t>
         </is>
       </c>
     </row>
@@ -2386,11 +2811,11 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Giovanni Freitas Pereira</t>
+          <t>José Pereira</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -2399,7 +2824,12 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>577.443.230-09</t>
+          <t>387.534.220-82</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>673265849</t>
         </is>
       </c>
     </row>
@@ -2409,20 +2839,25 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Paulo Vieira</t>
+          <t>Andressa Araújo</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>572.074.200-05</t>
+          <t>034.553.240-61</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>598751231</t>
         </is>
       </c>
     </row>
@@ -2432,20 +2867,25 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Regina Moraes</t>
+          <t>Felipe Oliveira</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>027.700.850-69</t>
+          <t>225.260.130-20</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>764770013</t>
         </is>
       </c>
     </row>
@@ -2455,11 +2895,11 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Sérgio Mendes</t>
+          <t>Lucas Pereira</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -2468,7 +2908,12 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>549.265.000-94</t>
+          <t>983.596.850-02</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>914964494</t>
         </is>
       </c>
     </row>
@@ -2478,11 +2923,11 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Roberto Dias</t>
+          <t>Márcio Pinto</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -2491,7 +2936,12 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>949.447.530-55</t>
+          <t>767.336.390-92</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>090175832</t>
         </is>
       </c>
     </row>
@@ -2501,20 +2951,25 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Jéssica Sousa</t>
+          <t>Álvaro Moraes</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>498.854.390-05</t>
+          <t>784.094.600-33</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>635096112</t>
         </is>
       </c>
     </row>
@@ -2524,20 +2979,25 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Eduardo Lopes</t>
+          <t>Felipe Rocha Vieira</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Não-Binário</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>529.643.730-60</t>
+          <t>536.562.760-13</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>635100144</t>
         </is>
       </c>
     </row>
@@ -2547,20 +3007,25 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Alberto Araújo</t>
+          <t>Carolina Borges</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>998.879.540-80</t>
+          <t>239.673.130-00</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>333642339</t>
         </is>
       </c>
     </row>
@@ -2570,20 +3035,25 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Sandra Melo</t>
+          <t>José Melo</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>144.699.740-56</t>
+          <t>869.105.810-24</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>775383854</t>
         </is>
       </c>
     </row>
@@ -2593,11 +3063,11 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Larissa Moraes</t>
+          <t>Maria Pessoa</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -2606,7 +3076,12 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>263.488.890-25</t>
+          <t>476.877.430-08</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>894899381</t>
         </is>
       </c>
     </row>
@@ -2616,11 +3091,11 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Karla Lima</t>
+          <t>Márcia Fernandes</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -2629,7 +3104,12 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>856.443.660-49</t>
+          <t>305.062.030-77</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>306374980</t>
         </is>
       </c>
     </row>
@@ -2639,11 +3119,11 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Carla Pereira</t>
+          <t>Renata Fernandes</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
@@ -2652,7 +3132,12 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>783.669.390-22</t>
+          <t>767.780.810-74</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>869827608</t>
         </is>
       </c>
     </row>
@@ -2662,11 +3147,11 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Mariana Machado</t>
+          <t>Carolina Costa</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
@@ -2675,7 +3160,12 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>456.825.350-06</t>
+          <t>682.518.890-90</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>338407601</t>
         </is>
       </c>
     </row>
@@ -2685,11 +3175,11 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Luiza Araújo</t>
+          <t>Mariana Pereira Lima</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
@@ -2698,7 +3188,12 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>055.054.560-30</t>
+          <t>738.980.470-08</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>745712977</t>
         </is>
       </c>
     </row>
@@ -2708,11 +3203,11 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>André Carvalho Sousa</t>
+          <t>Pedro Barbosa</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
@@ -2721,7 +3216,12 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>595.307.030-66</t>
+          <t>913.607.600-75</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>765197050</t>
         </is>
       </c>
     </row>
@@ -2731,20 +3231,25 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Bianca Correia Nunes</t>
+          <t>Raul Pereira</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>564.388.270-10</t>
+          <t>341.074.790-72</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>214174707</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Gerador de Perfis v2.2.1
</commit_message>
<xml_diff>
--- a/perfis_generated_openpyxl.xlsx
+++ b/perfis_generated_openpyxl.xlsx
@@ -459,11 +459,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Márcia Dias Pires</t>
+          <t>Vanessa Pereira</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -472,12 +472,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>454.730.420-31</t>
+          <t>573.556.850-74</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>457480213</t>
+          <t>733948172</t>
         </is>
       </c>
     </row>
@@ -487,11 +487,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Isaac Moraes</t>
+          <t>Lucas Sousa</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -500,12 +500,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>731.736.010-41</t>
+          <t>424.115.000-41</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>718388663</t>
+          <t>446097128</t>
         </is>
       </c>
     </row>
@@ -515,25 +515,25 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Raul Barbosa Pereira</t>
+          <t>Jéssica Gomes</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>734.122.850-48</t>
+          <t>540.222.030-13</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>375740544</t>
+          <t>786049820</t>
         </is>
       </c>
     </row>
@@ -543,11 +543,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Felipe Campos Correia</t>
+          <t>Thiago Araújo Machado</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -556,12 +556,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>464.763.310-19</t>
+          <t>406.083.250-23</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>840482879</t>
+          <t>650899627</t>
         </is>
       </c>
     </row>
@@ -571,11 +571,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Rosana Sousa</t>
+          <t>Juliana Rodrigues</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -584,12 +584,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>888.499.980-40</t>
+          <t>745.226.150-00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>473030048</t>
+          <t>256246839</t>
         </is>
       </c>
     </row>
@@ -599,25 +599,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Thais Martins</t>
+          <t>Raul Nogueira</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>035.001.300-46</t>
+          <t>382.217.820-92</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>807669998</t>
+          <t>832735806</t>
         </is>
       </c>
     </row>
@@ -627,25 +627,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Priscila Sousa</t>
+          <t>Wagner Dias</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>249.074.070-92</t>
+          <t>481.335.490-43</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>215971588</t>
+          <t>224524198</t>
         </is>
       </c>
     </row>
@@ -655,25 +655,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Mariana Lopes</t>
+          <t>Daniel Monteiro</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>130.928.250-12</t>
+          <t>132.465.740-57</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>570050630</t>
+          <t>286067774</t>
         </is>
       </c>
     </row>
@@ -683,11 +683,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Felipe Pereira</t>
+          <t>Vitor Silva</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -696,12 +696,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>700.595.730-07</t>
+          <t>100.136.710-30</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>026607922</t>
+          <t>477888927</t>
         </is>
       </c>
     </row>
@@ -711,11 +711,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Ana Gomes</t>
+          <t>Ana Pereira</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -724,12 +724,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>954.247.220-08</t>
+          <t>537.767.770-60</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>770449243</t>
+          <t>624166680</t>
         </is>
       </c>
     </row>
@@ -739,25 +739,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Regina Costa</t>
+          <t>Vitor Sousa</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>235.961.870-95</t>
+          <t>157.866.610-40</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>584915628</t>
+          <t>851958920</t>
         </is>
       </c>
     </row>
@@ -767,11 +767,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Jessica Fernandes Correia</t>
+          <t>Andréa Nascimento</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -780,12 +780,12 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>520.539.070-02</t>
+          <t>331.271.210-67</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>060319223</t>
+          <t>331699124</t>
         </is>
       </c>
     </row>
@@ -795,25 +795,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Vanessa Vieira</t>
+          <t>Carlos Gonçalves Borges</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>385.240.980-23</t>
+          <t>220.438.540-97</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>516677012</t>
+          <t>167419138</t>
         </is>
       </c>
     </row>
@@ -823,25 +823,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Elaine Lopes</t>
+          <t>Geraldo Nogueira</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>578.423.140-55</t>
+          <t>019.197.160-09</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>982299166</t>
+          <t>689807493</t>
         </is>
       </c>
     </row>
@@ -851,11 +851,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Nathalia Carvalho</t>
+          <t>Laura Pires Mendes</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -864,12 +864,12 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>073.690.740-80</t>
+          <t>158.699.350-08</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>261015531</t>
+          <t>568319041</t>
         </is>
       </c>
     </row>
@@ -879,25 +879,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Pedro Nunes</t>
+          <t>Thais Pinto</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>331.416.900-06</t>
+          <t>442.036.710-51</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>821956850</t>
+          <t>547633245</t>
         </is>
       </c>
     </row>
@@ -907,11 +907,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>José Ramos Nogueira</t>
+          <t>Renato Pereira</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -920,12 +920,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>372.826.150-55</t>
+          <t>106.303.180-00</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>743077956</t>
+          <t>299682155</t>
         </is>
       </c>
     </row>
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Laura Cardoso</t>
+          <t>Felipe Lima</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>134.432.000-79</t>
+          <t>598.773.900-43</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>612255228</t>
+          <t>455598355</t>
         </is>
       </c>
     </row>
@@ -963,25 +963,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Elias Monteiro</t>
+          <t>Isabela Pereira</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>946.794.820-60</t>
+          <t>733.047.230-13</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>290056748</t>
+          <t>457312888</t>
         </is>
       </c>
     </row>
@@ -991,25 +991,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Mariana Carvalho</t>
+          <t>Raul Carvalho</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>304.839.560-15</t>
+          <t>276.936.930-09</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>375496809</t>
+          <t>727150700</t>
         </is>
       </c>
     </row>
@@ -1019,25 +1019,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Diego Pereira Araújo</t>
+          <t>Tatiana Carvalho</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>498.409.200-90</t>
+          <t>415.980.460-80</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>167582780</t>
+          <t>341894667</t>
         </is>
       </c>
     </row>
@@ -1047,25 +1047,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Ana Pereira</t>
+          <t>Renato Lima</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>064.624.610-04</t>
+          <t>092.968.060-03</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>252755803</t>
+          <t>729449797</t>
         </is>
       </c>
     </row>
@@ -1075,25 +1075,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>João Carvalho</t>
+          <t>Mônica Fernandes Freitas</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>465.071.140-14</t>
+          <t>132.982.850-05</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>787197619</t>
+          <t>773615179</t>
         </is>
       </c>
     </row>
@@ -1103,11 +1103,11 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Gilberto Fernandes</t>
+          <t>Thiago Martins Correia</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1116,12 +1116,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>162.037.980-53</t>
+          <t>389.907.390-80</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>048896358</t>
+          <t>549912585</t>
         </is>
       </c>
     </row>
@@ -1131,7 +1131,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Rosana Pinto</t>
+          <t>Amanda Cavalcanti</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -1144,12 +1144,12 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804.864.460-69</t>
+          <t>754.470.500-57</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>900973832</t>
+          <t>179290943</t>
         </is>
       </c>
     </row>
@@ -1159,11 +1159,11 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Miguel Vieira</t>
+          <t>Sergio Mendes</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1172,12 +1172,12 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>031.895.000-61</t>
+          <t>199.544.060-42</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>842145565</t>
+          <t>583740282</t>
         </is>
       </c>
     </row>
@@ -1187,25 +1187,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Alexandre Rodrigues Nunes</t>
+          <t>Patrícia Andrade Rocha</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>694.366.080-20</t>
+          <t>628.826.310-90</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>746803141</t>
+          <t>798926152</t>
         </is>
       </c>
     </row>
@@ -1215,25 +1215,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Fábio Ramos</t>
+          <t>Eduarda Correia</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>612.312.490-05</t>
+          <t>186.257.350-61</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>794419543</t>
+          <t>215369521</t>
         </is>
       </c>
     </row>
@@ -1243,25 +1243,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Álvaro Lima</t>
+          <t>Ana Fernandes</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>972.260.190-35</t>
+          <t>840.554.340-65</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>114509439</t>
+          <t>838682997</t>
         </is>
       </c>
     </row>
@@ -1271,11 +1271,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Natália Freitas</t>
+          <t>Isabela Azevedo</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1284,12 +1284,12 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>168.919.910-56</t>
+          <t>713.489.240-98</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>122206954</t>
+          <t>398362527</t>
         </is>
       </c>
     </row>
@@ -1299,11 +1299,11 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Thais Melo</t>
+          <t>Mariana Pereira</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1312,12 +1312,12 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>880.239.540-32</t>
+          <t>428.452.310-40</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>299487657</t>
+          <t>038576566</t>
         </is>
       </c>
     </row>
@@ -1327,25 +1327,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Isabela Oliveira</t>
+          <t>Alberto Ribeira</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>603.222.170-91</t>
+          <t>895.761.560-17</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>139423656</t>
+          <t>478253051</t>
         </is>
       </c>
     </row>
@@ -1355,11 +1355,11 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Mariana Moraes</t>
+          <t>Camila Almeida</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1368,12 +1368,12 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>596.635.520-77</t>
+          <t>655.782.830-47</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>388024000</t>
+          <t>970503807</t>
         </is>
       </c>
     </row>
@@ -1383,11 +1383,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Valéria Carvalho</t>
+          <t>Tânia Barbosa Freitas</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1396,12 +1396,12 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>751.568.220-53</t>
+          <t>352.616.340-59</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>452742551</t>
+          <t>362135285</t>
         </is>
       </c>
     </row>
@@ -1411,11 +1411,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Juliana Oliveira Dias</t>
+          <t>Larissa Barros</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1424,12 +1424,12 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>070.093.130-91</t>
+          <t>167.372.260-19</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>857115097</t>
+          <t>131914646</t>
         </is>
       </c>
     </row>
@@ -1439,25 +1439,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Leticia Barbosa</t>
+          <t>Giovanni Ferreira</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>536.448.240-53</t>
+          <t>602.727.880-31</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>711540677</t>
+          <t>077158536</t>
         </is>
       </c>
     </row>
@@ -1467,25 +1467,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Leandro Nogueira Correia</t>
+          <t>Priscila Rodrigues Dias</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>201.951.320-09</t>
+          <t>597.188.150-74</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>280636763</t>
+          <t>567210217</t>
         </is>
       </c>
     </row>
@@ -1495,11 +1495,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Sandra Mendes Carvalho</t>
+          <t>Brenda Silveira</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1508,12 +1508,12 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>355.089.240-35</t>
+          <t>759.865.750-59</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>741495615</t>
+          <t>764559849</t>
         </is>
       </c>
     </row>
@@ -1523,11 +1523,11 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Patrícia Gouveia</t>
+          <t>Rafaela Ribeiro</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -1536,12 +1536,12 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>088.859.160-82</t>
+          <t>571.720.020-08</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>244913470</t>
+          <t>606735190</t>
         </is>
       </c>
     </row>
@@ -1551,25 +1551,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Simone Lopes</t>
+          <t>Renato Fernandes</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Não-Binário</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>128.180.470-30</t>
+          <t>437.155.560-80</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>953229688</t>
+          <t>042528214</t>
         </is>
       </c>
     </row>
@@ -1579,25 +1579,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Carlos Pires Dias</t>
+          <t>Thais Machado</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>382.751.550-53</t>
+          <t>777.535.500-04</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>244071353</t>
+          <t>472195552</t>
         </is>
       </c>
     </row>
@@ -1607,11 +1607,11 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Vitor Silveira</t>
+          <t>Alexandre Ferreira</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -1620,12 +1620,12 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>189.800.700-47</t>
+          <t>834.546.770-92</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>232713647</t>
+          <t>055938423</t>
         </is>
       </c>
     </row>
@@ -1635,25 +1635,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Alberto Barros</t>
+          <t>Larissa Ribeiro</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>277.193.980-09</t>
+          <t>032.019.360-81</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>387893829</t>
+          <t>756145745</t>
         </is>
       </c>
     </row>
@@ -1663,11 +1663,11 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Priscila Dias</t>
+          <t>Cátia Fernandes</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -1676,12 +1676,12 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>850.966.420-03</t>
+          <t>059.654.640-88</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>449182893</t>
+          <t>480213014</t>
         </is>
       </c>
     </row>
@@ -1691,11 +1691,11 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Luciano Lopes</t>
+          <t>Antônio Melo</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -1704,12 +1704,12 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>831.867.340-96</t>
+          <t>421.595.160-74</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>057502054</t>
+          <t>757223588</t>
         </is>
       </c>
     </row>
@@ -1719,25 +1719,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Luis Lima Gouveia</t>
+          <t>Laura Costa</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>559.979.500-42</t>
+          <t>417.796.470-00</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>546802468</t>
+          <t>129317238</t>
         </is>
       </c>
     </row>
@@ -1747,11 +1747,11 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Sergio Carvalho</t>
+          <t>Fábio Machado</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -1760,12 +1760,12 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>309.926.970-00</t>
+          <t>232.899.150-50</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>292559043</t>
+          <t>304532548</t>
         </is>
       </c>
     </row>
@@ -1775,25 +1775,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Juliana Ferreira Vieira</t>
+          <t>Elias Castro</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>096.588.340-00</t>
+          <t>705.041.870-66</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>908656150</t>
+          <t>200334799</t>
         </is>
       </c>
     </row>
@@ -1803,25 +1803,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Karla Ferreira</t>
+          <t>Fernando Mendes</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>978.118.970-32</t>
+          <t>610.621.770-02</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>916408101</t>
+          <t>520414693</t>
         </is>
       </c>
     </row>
@@ -1831,11 +1831,11 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Raul Fernandes</t>
+          <t>André Martins</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -1844,12 +1844,12 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>478.199.540-35</t>
+          <t>445.282.770-50</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>623764319</t>
+          <t>526827204</t>
         </is>
       </c>
     </row>
@@ -1859,11 +1859,11 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Carla Freitas</t>
+          <t>Eduarda Campos</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -1872,12 +1872,12 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>155.197.750-87</t>
+          <t>275.595.990-87</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>024109830</t>
+          <t>663774560</t>
         </is>
       </c>
     </row>
@@ -1887,25 +1887,25 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Patrícia Oliveira</t>
+          <t>Bruno Barbosa</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>287.636.970-25</t>
+          <t>632.919.140-90</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>418403233</t>
+          <t>402928418</t>
         </is>
       </c>
     </row>
@@ -1915,11 +1915,11 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Caio Lopes</t>
+          <t>Ronaldo Ferreira</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -1928,12 +1928,12 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>223.362.740-78</t>
+          <t>252.132.350-00</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>286796187</t>
+          <t>804111842</t>
         </is>
       </c>
     </row>
@@ -1943,25 +1943,25 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Ana Rodrigues</t>
+          <t>Raul Nogueira</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Não-Binário</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>245.758.110-92</t>
+          <t>448.128.100-60</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>513688306</t>
+          <t>990440190</t>
         </is>
       </c>
     </row>
@@ -1971,11 +1971,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Simone Dias</t>
+          <t>Flávia Nogueira Mendes</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -1984,12 +1984,12 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>552.835.850-77</t>
+          <t>403.056.770-39</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>053619195</t>
+          <t>031421887</t>
         </is>
       </c>
     </row>
@@ -1999,25 +1999,25 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>André Ramos</t>
+          <t>Mônica Lima</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>273.740.030-99</t>
+          <t>453.721.640-93</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>243745272</t>
+          <t>360277713</t>
         </is>
       </c>
     </row>
@@ -2027,11 +2027,11 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Roberta Costa</t>
+          <t>Ana Nascimento</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -2040,12 +2040,12 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>734.318.960-30</t>
+          <t>470.741.260-20</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>607822680</t>
+          <t>339183864</t>
         </is>
       </c>
     </row>
@@ -2055,25 +2055,25 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Armando Castro</t>
+          <t>Karla Costa Nogueira</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>494.679.480-87</t>
+          <t>226.776.570-58</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>894400711</t>
+          <t>693208528</t>
         </is>
       </c>
     </row>
@@ -2083,11 +2083,11 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Lucas Borges</t>
+          <t>Arnaldo Nascimento</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -2096,12 +2096,12 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>071.524.640-22</t>
+          <t>195.881.610-88</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>821110625</t>
+          <t>009154245</t>
         </is>
       </c>
     </row>
@@ -2111,25 +2111,25 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Samuel Ferreira</t>
+          <t>Tânia Cardoso</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>863.859.560-32</t>
+          <t>069.900.770-42</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>031551496</t>
+          <t>972038591</t>
         </is>
       </c>
     </row>
@@ -2139,25 +2139,25 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Guilherme Nunes</t>
+          <t>Natália Gomes Sousa</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>630.573.300-70</t>
+          <t>720.833.550-83</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>700093933</t>
+          <t>091669710</t>
         </is>
       </c>
     </row>
@@ -2167,11 +2167,11 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Samuel Silva</t>
+          <t>Fábio Ramos</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -2180,12 +2180,12 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>510.045.570-51</t>
+          <t>907.146.810-08</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>701802412</t>
+          <t>699537427</t>
         </is>
       </c>
     </row>
@@ -2195,25 +2195,25 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Ronaldo Moraes Campos</t>
+          <t>Renata Nascimento</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>450.616.830-56</t>
+          <t>410.459.510-13</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>268202430</t>
+          <t>322529750</t>
         </is>
       </c>
     </row>
@@ -2223,25 +2223,25 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Carla Martins</t>
+          <t>João Cardoso</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>623.701.950-29</t>
+          <t>918.404.680-50</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>803609982</t>
+          <t>479738883</t>
         </is>
       </c>
     </row>
@@ -2251,25 +2251,25 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Antônio Azevedo</t>
+          <t>Eduarda Oliveira</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>513.981.970-84</t>
+          <t>867.798.620-02</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>396946790</t>
+          <t>313400855</t>
         </is>
       </c>
     </row>
@@ -2279,25 +2279,25 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Patrícia Martins</t>
+          <t>Alexandre Pires</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>580.065.400-04</t>
+          <t>295.662.160-25</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>697792646</t>
+          <t>922476815</t>
         </is>
       </c>
     </row>
@@ -2307,11 +2307,11 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Thiago Lopes</t>
+          <t>Fernando Lima</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -2320,12 +2320,12 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>637.793.110-70</t>
+          <t>773.363.250-17</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>123234102</t>
+          <t>488133997</t>
         </is>
       </c>
     </row>
@@ -2335,25 +2335,25 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Cristina Machado</t>
+          <t>Wagner Oliveira</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>113.391.740-22</t>
+          <t>631.430.530-62</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>778409891</t>
+          <t>750937445</t>
         </is>
       </c>
     </row>
@@ -2363,25 +2363,25 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Leticia Ferreira</t>
+          <t>Giovanni Freitas Nunes</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>394.850.440-70</t>
+          <t>183.637.640-51</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>530521551</t>
+          <t>941841318</t>
         </is>
       </c>
     </row>
@@ -2391,11 +2391,11 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Carlos Santana</t>
+          <t>Wagner Borges</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -2404,12 +2404,12 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>380.183.210-43</t>
+          <t>105.791.420-78</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>030598201</t>
+          <t>825152671</t>
         </is>
       </c>
     </row>
@@ -2419,25 +2419,25 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Simone Castro</t>
+          <t>Sebastião Gouveia</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>532.753.590-88</t>
+          <t>228.586.680-19</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>742256244</t>
+          <t>139716926</t>
         </is>
       </c>
     </row>
@@ -2447,25 +2447,25 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Sandra Araújo</t>
+          <t>Luis Freitas</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>280.065.700-60</t>
+          <t>152.393.530-85</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>258305407</t>
+          <t>368253582</t>
         </is>
       </c>
     </row>
@@ -2475,25 +2475,25 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Vicente Pereira</t>
+          <t>Eduarda Ferreira Azevedo</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>713.336.930-36</t>
+          <t>811.962.800-45</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>362217362</t>
+          <t>601834505</t>
         </is>
       </c>
     </row>
@@ -2503,11 +2503,11 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>João Nogueira</t>
+          <t>Isaac Rodrigues Melo</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -2516,12 +2516,12 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>180.264.990-50</t>
+          <t>257.058.920-98</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>410084933</t>
+          <t>634761580</t>
         </is>
       </c>
     </row>
@@ -2531,7 +2531,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Fernando Freitas</t>
+          <t>Helena Moraes</t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -2539,17 +2539,17 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>055.224.730-88</t>
+          <t>336.901.940-08</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>990514266</t>
+          <t>455024086</t>
         </is>
       </c>
     </row>
@@ -2559,25 +2559,25 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Alexandre Santos Carvalho</t>
+          <t>Isabela Silveira</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>531.384.050-96</t>
+          <t>126.799.030-99</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>935528450</t>
+          <t>339396190</t>
         </is>
       </c>
     </row>
@@ -2587,25 +2587,25 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Raul Ribeira</t>
+          <t>Isabela Freitas</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>645.485.780-80</t>
+          <t>265.294.600-55</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>847359135</t>
+          <t>268020424</t>
         </is>
       </c>
     </row>
@@ -2615,25 +2615,25 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Larissa Freitas Barbosa</t>
+          <t>Fernando Mendes</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>100.413.760-56</t>
+          <t>856.987.500-25</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>394664282</t>
+          <t>269170213</t>
         </is>
       </c>
     </row>
@@ -2643,25 +2643,25 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Leonardo Lima</t>
+          <t>Mônica Campos</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>246.284.410-49</t>
+          <t>863.815.870-08</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>801523246</t>
+          <t>285692449</t>
         </is>
       </c>
     </row>
@@ -2671,25 +2671,25 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Juliana Mendes Lopes</t>
+          <t>Samuel Carvalho</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>078.697.430-38</t>
+          <t>815.250.800-40</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>734159646</t>
+          <t>254994710</t>
         </is>
       </c>
     </row>
@@ -2699,11 +2699,11 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Karla Nogueira Borges</t>
+          <t>Simone Silveira Nogueira</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -2712,12 +2712,12 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>241.540.760-78</t>
+          <t>927.222.580-99</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>180984797</t>
+          <t>877561712</t>
         </is>
       </c>
     </row>
@@ -2727,11 +2727,11 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Karla Nascimento</t>
+          <t>Mariana Pessoa Santana</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -2740,12 +2740,12 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>563.704.670-06</t>
+          <t>025.201.700-50</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>386690200</t>
+          <t>053818628</t>
         </is>
       </c>
     </row>
@@ -2755,11 +2755,11 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Amanda Moraes</t>
+          <t>Vanessa Melo</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -2768,12 +2768,12 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>415.604.520-05</t>
+          <t>140.007.360-00</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>124078147</t>
+          <t>533092203</t>
         </is>
       </c>
     </row>
@@ -2783,25 +2783,25 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Ricardo Gonçalves</t>
+          <t>Larissa Azevedo</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>898.639.190-20</t>
+          <t>670.344.460-91</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>331894100</t>
+          <t>254036678</t>
         </is>
       </c>
     </row>
@@ -2811,25 +2811,25 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>José Pereira</t>
+          <t>Fernanda Vieira</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>387.534.220-82</t>
+          <t>589.791.920-88</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>673265849</t>
+          <t>812017920</t>
         </is>
       </c>
     </row>
@@ -2839,11 +2839,11 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Andressa Araújo</t>
+          <t>Cátia Ferreira</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -2852,12 +2852,12 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>034.553.240-61</t>
+          <t>252.070.010-60</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>598751231</t>
+          <t>966278774</t>
         </is>
       </c>
     </row>
@@ -2867,11 +2867,11 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Felipe Oliveira</t>
+          <t>Joaquim Sousa</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -2880,12 +2880,12 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>225.260.130-20</t>
+          <t>424.456.660-07</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>764770013</t>
+          <t>878590873</t>
         </is>
       </c>
     </row>
@@ -2895,25 +2895,25 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Lucas Pereira</t>
+          <t>Carla Rocha</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>983.596.850-02</t>
+          <t>899.963.030-71</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>914964494</t>
+          <t>827564588</t>
         </is>
       </c>
     </row>
@@ -2923,11 +2923,11 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Márcio Pinto</t>
+          <t>Sergio Melo Mendes</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -2936,12 +2936,12 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>767.336.390-92</t>
+          <t>492.610.890-97</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>090175832</t>
+          <t>455174342</t>
         </is>
       </c>
     </row>
@@ -2951,7 +2951,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Álvaro Moraes</t>
+          <t>Fernando Barros</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -2964,12 +2964,12 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>784.094.600-33</t>
+          <t>085.523.190-47</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>635096112</t>
+          <t>847440391</t>
         </is>
       </c>
     </row>
@@ -2979,25 +2979,25 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Felipe Rocha Vieira</t>
+          <t>Bianca Ferreira Lopes</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Não-Binário</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>536.562.760-13</t>
+          <t>705.602.390-84</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>635100144</t>
+          <t>472480730</t>
         </is>
       </c>
     </row>
@@ -3007,25 +3007,25 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Carolina Borges</t>
+          <t>César Gomes</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>239.673.130-00</t>
+          <t>577.211.410-79</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>333642339</t>
+          <t>428238221</t>
         </is>
       </c>
     </row>
@@ -3035,25 +3035,25 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>José Melo</t>
+          <t>Tatiana Vieira</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>869.105.810-24</t>
+          <t>314.473.860-35</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>775383854</t>
+          <t>021788148</t>
         </is>
       </c>
     </row>
@@ -3063,25 +3063,25 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Maria Pessoa</t>
+          <t>Caio Ferreira</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>476.877.430-08</t>
+          <t>122.148.880-55</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>894899381</t>
+          <t>772594530</t>
         </is>
       </c>
     </row>
@@ -3091,11 +3091,11 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Márcia Fernandes</t>
+          <t>Larissa Andrade Almeida</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -3104,12 +3104,12 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>305.062.030-77</t>
+          <t>047.665.010-04</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>306374980</t>
+          <t>786668406</t>
         </is>
       </c>
     </row>
@@ -3119,25 +3119,25 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Renata Fernandes</t>
+          <t>Thais Castro</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Não-Binário</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>767.780.810-74</t>
+          <t>021.954.790-43</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>869827608</t>
+          <t>938607547</t>
         </is>
       </c>
     </row>
@@ -3147,11 +3147,11 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Carolina Costa</t>
+          <t>Tatiana Castro</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
@@ -3160,12 +3160,12 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>682.518.890-90</t>
+          <t>981.322.230-12</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>338407601</t>
+          <t>278114263</t>
         </is>
       </c>
     </row>
@@ -3175,11 +3175,11 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Mariana Pereira Lima</t>
+          <t>Mônica Rocha</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
@@ -3188,12 +3188,12 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>738.980.470-08</t>
+          <t>571.773.620-70</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>745712977</t>
+          <t>402454742</t>
         </is>
       </c>
     </row>
@@ -3203,11 +3203,11 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Pedro Barbosa</t>
+          <t>Diego Andrade</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
@@ -3216,12 +3216,12 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>913.607.600-75</t>
+          <t>915.749.000-72</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>765197050</t>
+          <t>203243931</t>
         </is>
       </c>
     </row>
@@ -3231,11 +3231,11 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Raul Pereira</t>
+          <t>Paulo Pires</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
@@ -3244,12 +3244,12 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>341.074.790-72</t>
+          <t>494.619.360-01</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>214174707</t>
+          <t>786344960</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Gerador de Perfis v2.2.2
</commit_message>
<xml_diff>
--- a/perfis_generated_openpyxl.xlsx
+++ b/perfis_generated_openpyxl.xlsx
@@ -459,25 +459,25 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Vanessa Pereira</t>
+          <t>Antônio Vinícius Freitas Almeida Vieira</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>573.556.850-74</t>
+          <t>580.142.100-93</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>733948172</t>
+          <t>171876915</t>
         </is>
       </c>
     </row>
@@ -487,25 +487,25 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Lucas Sousa</t>
+          <t>Tatiana Nathalia Alves Gouveia</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>424.115.000-41</t>
+          <t>851.022.300-93</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>446097128</t>
+          <t>307282167</t>
         </is>
       </c>
     </row>
@@ -515,25 +515,25 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jéssica Gomes</t>
+          <t>Fernando Sousa</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>540.222.030-13</t>
+          <t>001.074.090-20</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>786049820</t>
+          <t>689587047</t>
         </is>
       </c>
     </row>
@@ -543,25 +543,25 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Thiago Araújo Machado</t>
+          <t>Vanessa Nunes</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>406.083.250-23</t>
+          <t>459.015.280-00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>650899627</t>
+          <t>228019713</t>
         </is>
       </c>
     </row>
@@ -571,25 +571,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Juliana Rodrigues</t>
+          <t>Giovanni Gonçalves</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>745.226.150-00</t>
+          <t>610.559.420-84</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>256246839</t>
+          <t>759159814</t>
         </is>
       </c>
     </row>
@@ -599,11 +599,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Raul Nogueira</t>
+          <t>Gilberto Sousa Gomes Machado</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -612,12 +612,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>382.217.820-92</t>
+          <t>944.188.900-84</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>832735806</t>
+          <t>585342779</t>
         </is>
       </c>
     </row>
@@ -627,25 +627,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Wagner Dias</t>
+          <t>Cátia Ribeira Silva</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>481.335.490-43</t>
+          <t>928.966.580-76</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>224524198</t>
+          <t>167761469</t>
         </is>
       </c>
     </row>
@@ -655,25 +655,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Daniel Monteiro</t>
+          <t>Brenda Nascimento</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>132.465.740-57</t>
+          <t>820.383.120-60</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>286067774</t>
+          <t>706929634</t>
         </is>
       </c>
     </row>
@@ -683,25 +683,25 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Vitor Silva</t>
+          <t>Simone Lorena Nascimento Sousa</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>100.136.710-30</t>
+          <t>469.016.680-31</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>477888927</t>
+          <t>282286920</t>
         </is>
       </c>
     </row>
@@ -711,25 +711,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Ana Pereira</t>
+          <t>Ricardo Campos</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>537.767.770-60</t>
+          <t>418.649.190-94</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>624166680</t>
+          <t>138324908</t>
         </is>
       </c>
     </row>
@@ -739,25 +739,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Vitor Sousa</t>
+          <t>Cecília Nascimento Santos</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>157.866.610-40</t>
+          <t>888.548.530-89</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>851958920</t>
+          <t>582210410</t>
         </is>
       </c>
     </row>
@@ -767,25 +767,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Andréa Nascimento</t>
+          <t>Caio Monteiro Almeida</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>331.271.210-67</t>
+          <t>382.771.680-20</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>331699124</t>
+          <t>698728810</t>
         </is>
       </c>
     </row>
@@ -795,25 +795,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Carlos Gonçalves Borges</t>
+          <t>Larissa Borges</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>220.438.540-97</t>
+          <t>613.486.820-51</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>167419138</t>
+          <t>441901447</t>
         </is>
       </c>
     </row>
@@ -823,25 +823,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Geraldo Nogueira</t>
+          <t>Brenda Correia</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>019.197.160-09</t>
+          <t>752.725.820-98</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>689807493</t>
+          <t>425035900</t>
         </is>
       </c>
     </row>
@@ -851,11 +851,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Laura Pires Mendes</t>
+          <t>Camila Nogueira Ferreira</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -864,12 +864,12 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>158.699.350-08</t>
+          <t>866.518.390-63</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>568319041</t>
+          <t>476693212</t>
         </is>
       </c>
     </row>
@@ -879,11 +879,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Thais Pinto</t>
+          <t>Aline Andressa Nogueira Barbosa Gouveia Ribeiro</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -892,12 +892,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>442.036.710-51</t>
+          <t>456.206.810-84</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>547633245</t>
+          <t>220193085</t>
         </is>
       </c>
     </row>
@@ -907,25 +907,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Renato Pereira</t>
+          <t>Andréa Cardoso</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>106.303.180-00</t>
+          <t>360.852.880-69</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>299682155</t>
+          <t>780056683</t>
         </is>
       </c>
     </row>
@@ -935,25 +935,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Felipe Lima</t>
+          <t>Mônica Ramos Lopes</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>598.773.900-43</t>
+          <t>195.376.800-88</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>455598355</t>
+          <t>648454239</t>
         </is>
       </c>
     </row>
@@ -963,25 +963,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Isabela Pereira</t>
+          <t>Fábio Fernandes Lopes</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>733.047.230-13</t>
+          <t>082.368.660-41</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>457312888</t>
+          <t>630761978</t>
         </is>
       </c>
     </row>
@@ -991,25 +991,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Raul Carvalho</t>
+          <t>Tânia Mônica Ferreira Moraes</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>276.936.930-09</t>
+          <t>037.431.400-47</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>727150700</t>
+          <t>623340765</t>
         </is>
       </c>
     </row>
@@ -1019,11 +1019,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Tatiana Carvalho</t>
+          <t>Juliana Leticia Silveira Andrade Monteiro Azevedo</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1032,12 +1032,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>415.980.460-80</t>
+          <t>665.529.400-25</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>341894667</t>
+          <t>437541527</t>
         </is>
       </c>
     </row>
@@ -1047,11 +1047,11 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Renato Lima</t>
+          <t>Bruno Felipe Santana</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -1060,12 +1060,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>092.968.060-03</t>
+          <t>413.061.990-00</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>729449797</t>
+          <t>846277190</t>
         </is>
       </c>
     </row>
@@ -1075,25 +1075,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Mônica Fernandes Freitas</t>
+          <t>Pedro Nascimento</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>132.982.850-05</t>
+          <t>078.053.840-45</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>773615179</t>
+          <t>598332169</t>
         </is>
       </c>
     </row>
@@ -1103,11 +1103,11 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Thiago Martins Correia</t>
+          <t>Hugo Nunes Martins</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1116,12 +1116,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>389.907.390-80</t>
+          <t>136.167.640-09</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>549912585</t>
+          <t>515222218</t>
         </is>
       </c>
     </row>
@@ -1131,25 +1131,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Amanda Cavalcanti</t>
+          <t>Leonardo Pereira Andrade</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>754.470.500-57</t>
+          <t>925.376.840-10</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>179290943</t>
+          <t>691874218</t>
         </is>
       </c>
     </row>
@@ -1159,11 +1159,11 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Sergio Mendes</t>
+          <t>Roberto Carlos Santos Oliveira</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1172,12 +1172,12 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>199.544.060-42</t>
+          <t>095.476.290-85</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>583740282</t>
+          <t>983201164</t>
         </is>
       </c>
     </row>
@@ -1187,11 +1187,11 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Patrícia Andrade Rocha</t>
+          <t>Brenda Lima</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1200,12 +1200,12 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>628.826.310-90</t>
+          <t>067.683.930-49</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>798926152</t>
+          <t>752887215</t>
         </is>
       </c>
     </row>
@@ -1215,25 +1215,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Eduarda Correia</t>
+          <t>Fernando Pereira</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>186.257.350-61</t>
+          <t>286.937.800-93</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>215369521</t>
+          <t>225625638</t>
         </is>
       </c>
     </row>
@@ -1243,25 +1243,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Ana Fernandes</t>
+          <t>Vitor Cardoso Gomes</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>840.554.340-65</t>
+          <t>713.506.330-97</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>838682997</t>
+          <t>121676050</t>
         </is>
       </c>
     </row>
@@ -1271,11 +1271,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Isabela Azevedo</t>
+          <t>Carolina Santos Ferreira</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1284,12 +1284,12 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>713.489.240-98</t>
+          <t>423.080.910-70</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>398362527</t>
+          <t>605235240</t>
         </is>
       </c>
     </row>
@@ -1299,25 +1299,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Mariana Pereira</t>
+          <t>Thiago Barros Ramos</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>428.452.310-40</t>
+          <t>038.415.010-10</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>038576566</t>
+          <t>991594571</t>
         </is>
       </c>
     </row>
@@ -1327,25 +1327,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Alberto Ribeira</t>
+          <t>Priscila Mariana Gomes Mendes</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>895.761.560-17</t>
+          <t>881.980.250-30</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>478253051</t>
+          <t>346740872</t>
         </is>
       </c>
     </row>
@@ -1355,25 +1355,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Camila Almeida</t>
+          <t>Thiago Pinto</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>655.782.830-47</t>
+          <t>219.770.410-94</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>970503807</t>
+          <t>640675680</t>
         </is>
       </c>
     </row>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Tânia Barbosa Freitas</t>
+          <t>Ana Ferreira</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -1396,12 +1396,12 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>352.616.340-59</t>
+          <t>361.784.010-86</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>362135285</t>
+          <t>919300846</t>
         </is>
       </c>
     </row>
@@ -1411,25 +1411,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Larissa Barros</t>
+          <t>Wagner Roberto Nunes Freitas</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>167.372.260-19</t>
+          <t>455.586.170-12</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>131914646</t>
+          <t>052307560</t>
         </is>
       </c>
     </row>
@@ -1439,25 +1439,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Giovanni Ferreira</t>
+          <t>Renata Rocha Santana</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>602.727.880-31</t>
+          <t>765.908.170-57</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>077158536</t>
+          <t>447687078</t>
         </is>
       </c>
     </row>
@@ -1467,25 +1467,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Priscila Rodrigues Dias</t>
+          <t>Eduardo Daniel Ribeiro Ferreira</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>597.188.150-74</t>
+          <t>079.298.000-08</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>567210217</t>
+          <t>544922497</t>
         </is>
       </c>
     </row>
@@ -1495,25 +1495,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Brenda Silveira</t>
+          <t>Luciano Ramos</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>759.865.750-59</t>
+          <t>242.672.510-96</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>764559849</t>
+          <t>686827341</t>
         </is>
       </c>
     </row>
@@ -1523,11 +1523,11 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Rafaela Ribeiro</t>
+          <t>Valéria Rosana Moraes Sousa Fernandes</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -1536,12 +1536,12 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>571.720.020-08</t>
+          <t>011.554.100-41</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>606735190</t>
+          <t>654197087</t>
         </is>
       </c>
     </row>
@@ -1551,25 +1551,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Renato Fernandes</t>
+          <t>José Vieira</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Não-Binário</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>437.155.560-80</t>
+          <t>201.797.340-83</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>042528214</t>
+          <t>455800045</t>
         </is>
       </c>
     </row>
@@ -1579,11 +1579,11 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Thais Machado</t>
+          <t>Andréa Silva</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -1592,12 +1592,12 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>777.535.500-04</t>
+          <t>747.663.460-84</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>472195552</t>
+          <t>575489396</t>
         </is>
       </c>
     </row>
@@ -1607,25 +1607,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Alexandre Ferreira</t>
+          <t>Ana Fernandes Melo</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>834.546.770-92</t>
+          <t>816.911.850-60</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>055938423</t>
+          <t>581477092</t>
         </is>
       </c>
     </row>
@@ -1635,11 +1635,11 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Larissa Ribeiro</t>
+          <t>Larissa Sousa Gouveia</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -1648,12 +1648,12 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>032.019.360-81</t>
+          <t>925.827.440-77</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>756145745</t>
+          <t>248166578</t>
         </is>
       </c>
     </row>
@@ -1663,11 +1663,11 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Cátia Fernandes</t>
+          <t>Amanda Gomes</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -1676,12 +1676,12 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>059.654.640-88</t>
+          <t>646.319.270-89</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>480213014</t>
+          <t>062778093</t>
         </is>
       </c>
     </row>
@@ -1691,11 +1691,11 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Antônio Melo</t>
+          <t>Luis Alves Nascimento Araújo</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -1704,12 +1704,12 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>421.595.160-74</t>
+          <t>678.050.010-06</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>757223588</t>
+          <t>739601132</t>
         </is>
       </c>
     </row>
@@ -1719,25 +1719,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Laura Costa</t>
+          <t>Eduardo Nunes Andrade</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>417.796.470-00</t>
+          <t>436.459.470-94</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>129317238</t>
+          <t>179550775</t>
         </is>
       </c>
     </row>
@@ -1747,11 +1747,11 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Fábio Machado</t>
+          <t>Wagner Carvalho Lima</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -1760,12 +1760,12 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>232.899.150-50</t>
+          <t>964.217.590-84</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>304532548</t>
+          <t>528640000</t>
         </is>
       </c>
     </row>
@@ -1775,11 +1775,11 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Elias Castro</t>
+          <t>Daniel Ramos Azevedo Castro</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -1788,12 +1788,12 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>705.041.870-66</t>
+          <t>815.437.740-32</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>200334799</t>
+          <t>787344909</t>
         </is>
       </c>
     </row>
@@ -1803,25 +1803,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Fernando Mendes</t>
+          <t>Mariana Pereira</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>610.621.770-02</t>
+          <t>140.291.380-04</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>520414693</t>
+          <t>799419547</t>
         </is>
       </c>
     </row>
@@ -1831,25 +1831,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>André Martins</t>
+          <t>Andressa Carvalho Mendes</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>445.282.770-50</t>
+          <t>247.532.330-22</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>526827204</t>
+          <t>972493151</t>
         </is>
       </c>
     </row>
@@ -1859,25 +1859,25 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Eduarda Campos</t>
+          <t>Geraldo Lima Sousa</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>275.595.990-87</t>
+          <t>044.676.900-26</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>663774560</t>
+          <t>874729375</t>
         </is>
       </c>
     </row>
@@ -1887,25 +1887,25 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Bruno Barbosa</t>
+          <t>Tatiana Ferreira Fernandes</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>632.919.140-90</t>
+          <t>529.651.810-16</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>402928418</t>
+          <t>669592147</t>
         </is>
       </c>
     </row>
@@ -1915,25 +1915,25 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Ronaldo Ferreira</t>
+          <t>Bianca Rodrigues Ribeira</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>252.132.350-00</t>
+          <t>285.878.610-00</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>804111842</t>
+          <t>165717972</t>
         </is>
       </c>
     </row>
@@ -1943,25 +1943,25 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Raul Nogueira</t>
+          <t>Thais Juliana Silva Cardoso</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>448.128.100-60</t>
+          <t>545.916.340-43</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>990440190</t>
+          <t>885236608</t>
         </is>
       </c>
     </row>
@@ -1971,11 +1971,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Flávia Nogueira Mendes</t>
+          <t>Sandra Márcia Borges Barbosa Cardoso Lopes</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -1984,12 +1984,12 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>403.056.770-39</t>
+          <t>674.217.950-30</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>031421887</t>
+          <t>076900874</t>
         </is>
       </c>
     </row>
@@ -1999,11 +1999,11 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Mônica Lima</t>
+          <t>Lorena Gomes Rocha</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -2012,12 +2012,12 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>453.721.640-93</t>
+          <t>226.148.900-57</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>360277713</t>
+          <t>828161476</t>
         </is>
       </c>
     </row>
@@ -2027,11 +2027,11 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Ana Nascimento</t>
+          <t>Simone Pinto</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -2040,12 +2040,12 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>470.741.260-20</t>
+          <t>484.646.630-21</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>339183864</t>
+          <t>837491626</t>
         </is>
       </c>
     </row>
@@ -2055,11 +2055,11 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Karla Costa Nogueira</t>
+          <t>Amanda Lopes Sousa</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -2068,12 +2068,12 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>226.776.570-58</t>
+          <t>452.288.700-08</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>693208528</t>
+          <t>166671450</t>
         </is>
       </c>
     </row>
@@ -2083,11 +2083,11 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Arnaldo Nascimento</t>
+          <t>Arnaldo Pereira</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -2096,12 +2096,12 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>195.881.610-88</t>
+          <t>974.718.070-75</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>009154245</t>
+          <t>194310036</t>
         </is>
       </c>
     </row>
@@ -2111,7 +2111,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Tânia Cardoso</t>
+          <t>Amanda Barros</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -2124,12 +2124,12 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>069.900.770-42</t>
+          <t>417.694.370-02</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>972038591</t>
+          <t>555122713</t>
         </is>
       </c>
     </row>
@@ -2139,11 +2139,11 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Natália Gomes Sousa</t>
+          <t>Bianca Dias</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -2152,12 +2152,12 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>720.833.550-83</t>
+          <t>709.053.850-80</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>091669710</t>
+          <t>362984744</t>
         </is>
       </c>
     </row>
@@ -2167,25 +2167,25 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Fábio Ramos</t>
+          <t>Bianca Melo Oliveira</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>907.146.810-08</t>
+          <t>709.701.630-29</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>699537427</t>
+          <t>958251390</t>
         </is>
       </c>
     </row>
@@ -2195,11 +2195,11 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Renata Nascimento</t>
+          <t>Larissa Amanda Lima</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -2208,12 +2208,12 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>410.459.510-13</t>
+          <t>687.201.150-59</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>322529750</t>
+          <t>126182543</t>
         </is>
       </c>
     </row>
@@ -2223,11 +2223,11 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>João Cardoso</t>
+          <t>Luis Machado Dias</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -2236,12 +2236,12 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>918.404.680-50</t>
+          <t>295.693.230-60</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>479738883</t>
+          <t>685127585</t>
         </is>
       </c>
     </row>
@@ -2251,25 +2251,25 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Eduarda Oliveira</t>
+          <t>Caio Carlos Barbosa Correia Lima</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>867.798.620-02</t>
+          <t>027.358.540-19</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>313400855</t>
+          <t>575659158</t>
         </is>
       </c>
     </row>
@@ -2279,25 +2279,25 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Alexandre Pires</t>
+          <t>Mariana Carvalho</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>295.662.160-25</t>
+          <t>796.146.210-44</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>922476815</t>
+          <t>471883300</t>
         </is>
       </c>
     </row>
@@ -2307,25 +2307,25 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Fernando Lima</t>
+          <t>Regina Renata Freitas Correia</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>773.363.250-17</t>
+          <t>313.845.910-28</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>488133997</t>
+          <t>183043895</t>
         </is>
       </c>
     </row>
@@ -2335,11 +2335,11 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Wagner Oliveira</t>
+          <t>Ronaldo Alves Ribeiro</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -2348,12 +2348,12 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>631.430.530-62</t>
+          <t>696.016.480-03</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>750937445</t>
+          <t>160081716</t>
         </is>
       </c>
     </row>
@@ -2363,25 +2363,25 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Giovanni Freitas Nunes</t>
+          <t>Mônica Vieira Gomes Fernandes</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>183.637.640-51</t>
+          <t>664.847.530-75</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>941841318</t>
+          <t>964510658</t>
         </is>
       </c>
     </row>
@@ -2391,11 +2391,11 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Wagner Borges</t>
+          <t>Gilberto Sousa Vieira</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -2404,12 +2404,12 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>105.791.420-78</t>
+          <t>401.601.800-58</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>825152671</t>
+          <t>376016622</t>
         </is>
       </c>
     </row>
@@ -2419,25 +2419,25 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Sebastião Gouveia</t>
+          <t>Cecília Sandra Cavalcanti Lopes Ribeira</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>228.586.680-19</t>
+          <t>507.073.040-16</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>139716926</t>
+          <t>123757138</t>
         </is>
       </c>
     </row>
@@ -2447,25 +2447,25 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Luis Freitas</t>
+          <t>Jessica Larissa Machado Santana</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>152.393.530-85</t>
+          <t>858.233.020-02</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>368253582</t>
+          <t>455806048</t>
         </is>
       </c>
     </row>
@@ -2475,11 +2475,11 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Eduarda Ferreira Azevedo</t>
+          <t>Eduarda Cavalcanti Cavalcanti</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -2488,12 +2488,12 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>811.962.800-45</t>
+          <t>431.897.740-48</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>601834505</t>
+          <t>670110199</t>
         </is>
       </c>
     </row>
@@ -2503,25 +2503,25 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Isaac Rodrigues Melo</t>
+          <t>Elias Eduardo Lopes Lima</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Não-Binário</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>257.058.920-98</t>
+          <t>167.230.080-06</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>634761580</t>
+          <t>026107380</t>
         </is>
       </c>
     </row>
@@ -2531,11 +2531,11 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Helena Moraes</t>
+          <t>Vanessa Gomes Machado</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -2544,12 +2544,12 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>336.901.940-08</t>
+          <t>692.771.170-87</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>455024086</t>
+          <t>924379998</t>
         </is>
       </c>
     </row>
@@ -2559,25 +2559,25 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Isabela Silveira</t>
+          <t>Lucas Diego Monteiro</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>126.799.030-99</t>
+          <t>338.298.470-92</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>339396190</t>
+          <t>846845006</t>
         </is>
       </c>
     </row>
@@ -2587,11 +2587,11 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Isabela Freitas</t>
+          <t>Simone Campos Santana</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -2600,12 +2600,12 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>265.294.600-55</t>
+          <t>535.481.650-52</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>268020424</t>
+          <t>997953270</t>
         </is>
       </c>
     </row>
@@ -2615,25 +2615,25 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Fernando Mendes</t>
+          <t>Thais Nascimento</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>856.987.500-25</t>
+          <t>446.669.530-00</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>269170213</t>
+          <t>471061931</t>
         </is>
       </c>
     </row>
@@ -2643,11 +2643,11 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Mônica Campos</t>
+          <t>Thais Carvalho Dias Fernandes Mendes</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -2656,12 +2656,12 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>863.815.870-08</t>
+          <t>413.602.630-71</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>285692449</t>
+          <t>127211340</t>
         </is>
       </c>
     </row>
@@ -2671,11 +2671,11 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Samuel Carvalho</t>
+          <t>Giovanni Pinto</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -2684,12 +2684,12 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>815.250.800-40</t>
+          <t>726.060.550-20</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>254994710</t>
+          <t>501191920</t>
         </is>
       </c>
     </row>
@@ -2699,25 +2699,25 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Simone Silveira Nogueira</t>
+          <t>Elias Campos</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>927.222.580-99</t>
+          <t>617.544.010-23</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>877561712</t>
+          <t>986132474</t>
         </is>
       </c>
     </row>
@@ -2727,25 +2727,25 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Mariana Pessoa Santana</t>
+          <t>Carlos Campos Machado Ribeiro</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>025.201.700-50</t>
+          <t>270.888.210-44</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>053818628</t>
+          <t>414024556</t>
         </is>
       </c>
     </row>
@@ -2755,25 +2755,25 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Vanessa Melo</t>
+          <t>Mônica Gonçalves</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Não-Binário</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>140.007.360-00</t>
+          <t>111.467.300-55</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>533092203</t>
+          <t>430309056</t>
         </is>
       </c>
     </row>
@@ -2783,25 +2783,25 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Larissa Azevedo</t>
+          <t>Leonardo Fernandes Costa Pereira Oliveira</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>670.344.460-91</t>
+          <t>417.540.790-16</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>254036678</t>
+          <t>465763030</t>
         </is>
       </c>
     </row>
@@ -2811,25 +2811,25 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Fernanda Vieira</t>
+          <t>Bruno Vinícius Dias Carvalho</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>589.791.920-88</t>
+          <t>284.156.830-06</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>812017920</t>
+          <t>983323168</t>
         </is>
       </c>
     </row>
@@ -2839,25 +2839,25 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Cátia Ferreira</t>
+          <t>Joaquim Moraes Almeida Almeida Dias</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Não-Binário</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>252.070.010-60</t>
+          <t>148.542.460-73</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>966278774</t>
+          <t>070384721</t>
         </is>
       </c>
     </row>
@@ -2867,25 +2867,25 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Joaquim Sousa</t>
+          <t>Fernanda Aline Silveira Campos</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>424.456.660-07</t>
+          <t>643.936.650-58</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>878590873</t>
+          <t>104579994</t>
         </is>
       </c>
     </row>
@@ -2895,11 +2895,11 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Carla Rocha</t>
+          <t>Sandra Nascimento Pessoa</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -2908,12 +2908,12 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>899.963.030-71</t>
+          <t>229.902.260-01</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>827564588</t>
+          <t>019231081</t>
         </is>
       </c>
     </row>
@@ -2923,11 +2923,11 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Sergio Melo Mendes</t>
+          <t>Márcio Caio Sousa Alves</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -2936,12 +2936,12 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>492.610.890-97</t>
+          <t>249.598.230-11</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>455174342</t>
+          <t>905036710</t>
         </is>
       </c>
     </row>
@@ -2951,25 +2951,25 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Fernando Barros</t>
+          <t>Valéria Priscila Ferreira Rodrigues</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>085.523.190-47</t>
+          <t>060.576.620-75</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>847440391</t>
+          <t>573540454</t>
         </is>
       </c>
     </row>
@@ -2979,25 +2979,25 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Bianca Ferreira Lopes</t>
+          <t>Joaquim César Nunes</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>705.602.390-84</t>
+          <t>547.518.160-80</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>472480730</t>
+          <t>839946282</t>
         </is>
       </c>
     </row>
@@ -3007,25 +3007,25 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>César Gomes</t>
+          <t>Aline Barros</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>577.211.410-79</t>
+          <t>900.037.450-23</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>428238221</t>
+          <t>246882640</t>
         </is>
       </c>
     </row>
@@ -3035,11 +3035,11 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Tatiana Vieira</t>
+          <t>Rosana Freitas Dias</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -3048,12 +3048,12 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>314.473.860-35</t>
+          <t>875.453.660-00</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>021788148</t>
+          <t>587861300</t>
         </is>
       </c>
     </row>
@@ -3063,25 +3063,25 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Caio Ferreira</t>
+          <t>Andréa Barbosa Ferreira</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>122.148.880-55</t>
+          <t>116.712.740-40</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>772594530</t>
+          <t>418872736</t>
         </is>
       </c>
     </row>
@@ -3091,25 +3091,25 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Larissa Andrade Almeida</t>
+          <t>Alexandre Araújo Pereira Borges Campos</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>047.665.010-04</t>
+          <t>733.398.620-95</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>786668406</t>
+          <t>582744908</t>
         </is>
       </c>
     </row>
@@ -3119,25 +3119,25 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Thais Castro</t>
+          <t>Thiago Gonçalves Monteiro Pinto Gomes</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Não-Binário</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>021.954.790-43</t>
+          <t>053.470.570-76</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>938607547</t>
+          <t>571982242</t>
         </is>
       </c>
     </row>
@@ -3147,11 +3147,11 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Tatiana Castro</t>
+          <t>Helena Gouveia Ferreira</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
@@ -3160,12 +3160,12 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>981.322.230-12</t>
+          <t>560.066.620-94</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>278114263</t>
+          <t>672721285</t>
         </is>
       </c>
     </row>
@@ -3175,11 +3175,11 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Mônica Rocha</t>
+          <t>Tatiana Eduarda Nascimento Lopes</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
@@ -3188,12 +3188,12 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>571.773.620-70</t>
+          <t>659.408.630-86</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>402454742</t>
+          <t>692038329</t>
         </is>
       </c>
     </row>
@@ -3203,25 +3203,25 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Diego Andrade</t>
+          <t>Isabela Carla Mendes Sousa</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>915.749.000-72</t>
+          <t>745.467.290-65</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>203243931</t>
+          <t>768550623</t>
         </is>
       </c>
     </row>
@@ -3231,25 +3231,25 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Paulo Pires</t>
+          <t>Helena Mariana Pereira</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>494.619.360-01</t>
+          <t>997.026.760-45</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>786344960</t>
+          <t>494128944</t>
         </is>
       </c>
     </row>

</xml_diff>